<commit_message>
Add new company when the other one is filled
</commit_message>
<xml_diff>
--- a/src/output/results1.xlsx
+++ b/src/output/results1.xlsx
@@ -380,13 +380,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -397,13 +397,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
@@ -414,13 +414,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C5" t="n">
         <v>1.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
@@ -431,13 +431,13 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
@@ -448,13 +448,13 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="B7" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="C7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7" t="n">
         <v>0.0</v>
@@ -465,13 +465,13 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="B8" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="C8" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
@@ -482,13 +482,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="B9" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="C9" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="D9" t="n">
         <v>0.0</v>
@@ -499,13 +499,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="B10" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="C10" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="D10" t="n">
         <v>0.0</v>
@@ -516,30 +516,30 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>52.0</v>
+        <v>56.0</v>
       </c>
       <c r="B11" t="n">
-        <v>52.0</v>
+        <v>55.0</v>
       </c>
       <c r="C11" t="n">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="D11" t="n">
         <v>0.0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>70.0</v>
+        <v>67.0</v>
       </c>
       <c r="B12" t="n">
-        <v>69.0</v>
+        <v>66.0</v>
       </c>
       <c r="C12" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
       <c r="D12" t="n">
         <v>0.0</v>
@@ -550,1651 +550,1651 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>84.0</v>
+        <v>86.0</v>
       </c>
       <c r="B13" t="n">
         <v>83.0</v>
       </c>
       <c r="C13" t="n">
-        <v>14.0</v>
+        <v>19.0</v>
       </c>
       <c r="D13" t="n">
         <v>0.0</v>
       </c>
       <c r="E13" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>109.0</v>
+        <v>102.0</v>
       </c>
       <c r="B14" t="n">
-        <v>106.0</v>
+        <v>98.0</v>
       </c>
       <c r="C14" t="n">
-        <v>25.0</v>
+        <v>16.0</v>
       </c>
       <c r="D14" t="n">
         <v>0.0</v>
       </c>
       <c r="E14" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>143.0</v>
+        <v>115.0</v>
       </c>
       <c r="B15" t="n">
-        <v>139.0</v>
+        <v>107.0</v>
       </c>
       <c r="C15" t="n">
-        <v>34.0</v>
+        <v>13.0</v>
       </c>
       <c r="D15" t="n">
         <v>0.0</v>
       </c>
       <c r="E15" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>177.0</v>
+        <v>141.0</v>
       </c>
       <c r="B16" t="n">
-        <v>169.0</v>
+        <v>129.0</v>
       </c>
       <c r="C16" t="n">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E16" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>218.0</v>
+        <v>189.0</v>
       </c>
       <c r="B17" t="n">
-        <v>204.0</v>
+        <v>173.0</v>
       </c>
       <c r="C17" t="n">
-        <v>41.0</v>
+        <v>48.0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E17" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>273.0</v>
+        <v>229.0</v>
       </c>
       <c r="B18" t="n">
-        <v>247.0</v>
+        <v>205.0</v>
       </c>
       <c r="C18" t="n">
-        <v>55.0</v>
+        <v>40.0</v>
       </c>
       <c r="D18" t="n">
         <v>1.0</v>
       </c>
       <c r="E18" t="n">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>342.0</v>
+        <v>274.0</v>
       </c>
       <c r="B19" t="n">
-        <v>309.0</v>
+        <v>244.0</v>
       </c>
       <c r="C19" t="n">
-        <v>69.0</v>
+        <v>45.0</v>
       </c>
       <c r="D19" t="n">
         <v>1.0</v>
       </c>
       <c r="E19" t="n">
-        <v>32.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>429.0</v>
+        <v>343.0</v>
       </c>
       <c r="B20" t="n">
-        <v>385.0</v>
+        <v>307.0</v>
       </c>
       <c r="C20" t="n">
-        <v>87.0</v>
+        <v>69.0</v>
       </c>
       <c r="D20" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E20" t="n">
-        <v>42.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>516.0</v>
+        <v>422.0</v>
       </c>
       <c r="B21" t="n">
-        <v>460.0</v>
+        <v>378.0</v>
       </c>
       <c r="C21" t="n">
-        <v>87.0</v>
+        <v>79.0</v>
       </c>
       <c r="D21" t="n">
         <v>2.0</v>
       </c>
       <c r="E21" t="n">
-        <v>54.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>615.0</v>
+        <v>496.0</v>
       </c>
       <c r="B22" t="n">
-        <v>541.0</v>
+        <v>446.0</v>
       </c>
       <c r="C22" t="n">
-        <v>99.0</v>
+        <v>74.0</v>
       </c>
       <c r="D22" t="n">
         <v>2.0</v>
       </c>
       <c r="E22" t="n">
-        <v>72.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>751.0</v>
+        <v>591.0</v>
       </c>
       <c r="B23" t="n">
-        <v>661.0</v>
+        <v>523.0</v>
       </c>
       <c r="C23" t="n">
-        <v>136.0</v>
+        <v>95.0</v>
       </c>
       <c r="D23" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E23" t="n">
-        <v>88.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>878.0</v>
+        <v>701.0</v>
       </c>
       <c r="B24" t="n">
-        <v>760.0</v>
+        <v>605.0</v>
       </c>
       <c r="C24" t="n">
-        <v>127.0</v>
+        <v>110.0</v>
       </c>
       <c r="D24" t="n">
         <v>3.0</v>
       </c>
       <c r="E24" t="n">
-        <v>115.0</v>
+        <v>93.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1015.0</v>
+        <v>820.0</v>
       </c>
       <c r="B25" t="n">
-        <v>867.0</v>
+        <v>697.0</v>
       </c>
       <c r="C25" t="n">
-        <v>137.0</v>
+        <v>119.0</v>
       </c>
       <c r="D25" t="n">
         <v>3.0</v>
       </c>
       <c r="E25" t="n">
-        <v>145.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1190.0</v>
+        <v>942.0</v>
       </c>
       <c r="B26" t="n">
-        <v>1008.0</v>
+        <v>789.0</v>
       </c>
       <c r="C26" t="n">
-        <v>175.0</v>
+        <v>122.0</v>
       </c>
       <c r="D26" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E26" t="n">
-        <v>178.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1352.0</v>
+        <v>1089.0</v>
       </c>
       <c r="B27" t="n">
-        <v>1131.0</v>
+        <v>902.0</v>
       </c>
       <c r="C27" t="n">
-        <v>162.0</v>
+        <v>147.0</v>
       </c>
       <c r="D27" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E27" t="n">
-        <v>217.0</v>
+        <v>184.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1566.0</v>
+        <v>1263.0</v>
       </c>
       <c r="B28" t="n">
-        <v>1301.0</v>
+        <v>1048.0</v>
       </c>
       <c r="C28" t="n">
-        <v>214.0</v>
+        <v>174.0</v>
       </c>
       <c r="D28" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E28" t="n">
-        <v>261.0</v>
+        <v>212.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1844.0</v>
+        <v>1425.0</v>
       </c>
       <c r="B29" t="n">
-        <v>1532.0</v>
+        <v>1164.0</v>
       </c>
       <c r="C29" t="n">
-        <v>278.0</v>
+        <v>162.0</v>
       </c>
       <c r="D29" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E29" t="n">
-        <v>308.0</v>
+        <v>258.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2129.0</v>
+        <v>1642.0</v>
       </c>
       <c r="B30" t="n">
-        <v>1764.0</v>
+        <v>1336.0</v>
       </c>
       <c r="C30" t="n">
-        <v>285.0</v>
+        <v>217.0</v>
       </c>
       <c r="D30" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E30" t="n">
-        <v>361.0</v>
+        <v>303.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2482.0</v>
+        <v>1886.0</v>
       </c>
       <c r="B31" t="n">
-        <v>2048.0</v>
+        <v>1521.0</v>
       </c>
       <c r="C31" t="n">
-        <v>353.0</v>
+        <v>244.0</v>
       </c>
       <c r="D31" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E31" t="n">
-        <v>428.0</v>
+        <v>362.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2904.0</v>
+        <v>2188.0</v>
       </c>
       <c r="B32" t="n">
-        <v>2392.0</v>
+        <v>1746.0</v>
       </c>
       <c r="C32" t="n">
-        <v>422.0</v>
+        <v>302.0</v>
       </c>
       <c r="D32" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="E32" t="n">
-        <v>503.0</v>
+        <v>438.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3403.0</v>
+        <v>2526.0</v>
       </c>
       <c r="B33" t="n">
-        <v>2783.0</v>
+        <v>2007.0</v>
       </c>
       <c r="C33" t="n">
-        <v>499.0</v>
+        <v>338.0</v>
       </c>
       <c r="D33" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="E33" t="n">
-        <v>611.0</v>
+        <v>511.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>3885.0</v>
+        <v>2959.0</v>
       </c>
       <c r="B34" t="n">
-        <v>3145.0</v>
+        <v>2351.0</v>
       </c>
       <c r="C34" t="n">
-        <v>482.0</v>
+        <v>433.0</v>
       </c>
       <c r="D34" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="E34" t="n">
-        <v>730.0</v>
+        <v>596.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>4484.0</v>
+        <v>3411.0</v>
       </c>
       <c r="B35" t="n">
-        <v>3621.0</v>
+        <v>2710.0</v>
       </c>
       <c r="C35" t="n">
-        <v>599.0</v>
+        <v>452.0</v>
       </c>
       <c r="D35" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="E35" t="n">
-        <v>850.0</v>
+        <v>685.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5194.0</v>
+        <v>3970.0</v>
       </c>
       <c r="B36" t="n">
-        <v>4184.0</v>
+        <v>3149.0</v>
       </c>
       <c r="C36" t="n">
-        <v>710.0</v>
+        <v>559.0</v>
       </c>
       <c r="D36" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="E36" t="n">
-        <v>995.0</v>
+        <v>804.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>6032.0</v>
+        <v>4620.0</v>
       </c>
       <c r="B37" t="n">
-        <v>4844.0</v>
+        <v>3665.0</v>
       </c>
       <c r="C37" t="n">
-        <v>838.0</v>
+        <v>650.0</v>
       </c>
       <c r="D37" t="n">
-        <v>22.0</v>
+        <v>18.0</v>
       </c>
       <c r="E37" t="n">
-        <v>1166.0</v>
+        <v>937.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7083.0</v>
+        <v>5399.0</v>
       </c>
       <c r="B38" t="n">
-        <v>5703.0</v>
+        <v>4307.0</v>
       </c>
       <c r="C38" t="n">
-        <v>1051.0</v>
+        <v>779.0</v>
       </c>
       <c r="D38" t="n">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
       <c r="E38" t="n">
-        <v>1356.0</v>
+        <v>1073.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>8229.0</v>
+        <v>6351.0</v>
       </c>
       <c r="B39" t="n">
-        <v>6616.0</v>
+        <v>5085.0</v>
       </c>
       <c r="C39" t="n">
-        <v>1146.0</v>
+        <v>952.0</v>
       </c>
       <c r="D39" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="E39" t="n">
-        <v>1587.0</v>
+        <v>1244.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>9565.0</v>
+        <v>7351.0</v>
       </c>
       <c r="B40" t="n">
-        <v>7672.0</v>
+        <v>5899.0</v>
       </c>
       <c r="C40" t="n">
-        <v>1336.0</v>
+        <v>1000.0</v>
       </c>
       <c r="D40" t="n">
-        <v>28.0</v>
+        <v>22.0</v>
       </c>
       <c r="E40" t="n">
-        <v>1865.0</v>
+        <v>1430.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>11079.0</v>
+        <v>8503.0</v>
       </c>
       <c r="B41" t="n">
-        <v>8920.0</v>
+        <v>6833.0</v>
       </c>
       <c r="C41" t="n">
-        <v>1514.0</v>
+        <v>1152.0</v>
       </c>
       <c r="D41" t="n">
-        <v>29.0</v>
+        <v>27.0</v>
       </c>
       <c r="E41" t="n">
-        <v>2130.0</v>
+        <v>1643.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>12746.0</v>
+        <v>9795.0</v>
       </c>
       <c r="B42" t="n">
-        <v>10243.0</v>
+        <v>7892.0</v>
       </c>
       <c r="C42" t="n">
-        <v>1667.0</v>
+        <v>1292.0</v>
       </c>
       <c r="D42" t="n">
-        <v>36.0</v>
+        <v>30.0</v>
       </c>
       <c r="E42" t="n">
-        <v>2467.0</v>
+        <v>1873.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>14731.0</v>
+        <v>11266.0</v>
       </c>
       <c r="B43" t="n">
-        <v>11828.0</v>
+        <v>9054.0</v>
       </c>
       <c r="C43" t="n">
-        <v>1985.0</v>
+        <v>1471.0</v>
       </c>
       <c r="D43" t="n">
-        <v>44.0</v>
+        <v>32.0</v>
       </c>
       <c r="E43" t="n">
-        <v>2859.0</v>
+        <v>2180.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>16962.0</v>
+        <v>12956.0</v>
       </c>
       <c r="B44" t="n">
-        <v>13565.0</v>
+        <v>10383.0</v>
       </c>
       <c r="C44" t="n">
-        <v>2231.0</v>
+        <v>1690.0</v>
       </c>
       <c r="D44" t="n">
-        <v>49.0</v>
+        <v>40.0</v>
       </c>
       <c r="E44" t="n">
-        <v>3348.0</v>
+        <v>2533.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>19515.0</v>
+        <v>14976.0</v>
       </c>
       <c r="B45" t="n">
-        <v>15567.0</v>
+        <v>11962.0</v>
       </c>
       <c r="C45" t="n">
-        <v>2553.0</v>
+        <v>2020.0</v>
       </c>
       <c r="D45" t="n">
-        <v>54.0</v>
+        <v>46.0</v>
       </c>
       <c r="E45" t="n">
-        <v>3894.0</v>
+        <v>2968.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>22364.0</v>
+        <v>17219.0</v>
       </c>
       <c r="B46" t="n">
-        <v>17792.0</v>
+        <v>13708.0</v>
       </c>
       <c r="C46" t="n">
-        <v>2849.0</v>
+        <v>2243.0</v>
       </c>
       <c r="D46" t="n">
-        <v>66.0</v>
+        <v>52.0</v>
       </c>
       <c r="E46" t="n">
-        <v>4506.0</v>
+        <v>3459.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>25600.0</v>
+        <v>19752.0</v>
       </c>
       <c r="B47" t="n">
-        <v>20274.0</v>
+        <v>15662.0</v>
       </c>
       <c r="C47" t="n">
-        <v>3236.0</v>
+        <v>2533.0</v>
       </c>
       <c r="D47" t="n">
-        <v>77.0</v>
+        <v>69.0</v>
       </c>
       <c r="E47" t="n">
-        <v>5249.0</v>
+        <v>4021.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>29219.0</v>
+        <v>22577.0</v>
       </c>
       <c r="B48" t="n">
-        <v>23039.0</v>
+        <v>17808.0</v>
       </c>
       <c r="C48" t="n">
-        <v>3619.0</v>
+        <v>2825.0</v>
       </c>
       <c r="D48" t="n">
-        <v>90.0</v>
+        <v>81.0</v>
       </c>
       <c r="E48" t="n">
-        <v>6090.0</v>
+        <v>4688.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>33080.0</v>
+        <v>25769.0</v>
       </c>
       <c r="B49" t="n">
-        <v>25882.0</v>
+        <v>20256.0</v>
       </c>
       <c r="C49" t="n">
-        <v>3861.0</v>
+        <v>3192.0</v>
       </c>
       <c r="D49" t="n">
-        <v>101.0</v>
+        <v>99.0</v>
       </c>
       <c r="E49" t="n">
-        <v>7097.0</v>
+        <v>5414.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>37244.0</v>
+        <v>29240.0</v>
       </c>
       <c r="B50" t="n">
-        <v>28852.0</v>
+        <v>22879.0</v>
       </c>
       <c r="C50" t="n">
-        <v>4164.0</v>
+        <v>3471.0</v>
       </c>
       <c r="D50" t="n">
-        <v>114.0</v>
+        <v>111.0</v>
       </c>
       <c r="E50" t="n">
-        <v>8278.0</v>
+        <v>6250.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>41921.0</v>
+        <v>33255.0</v>
       </c>
       <c r="B51" t="n">
-        <v>32199.0</v>
+        <v>25882.0</v>
       </c>
       <c r="C51" t="n">
-        <v>4677.0</v>
+        <v>4015.0</v>
       </c>
       <c r="D51" t="n">
-        <v>142.0</v>
+        <v>121.0</v>
       </c>
       <c r="E51" t="n">
-        <v>9580.0</v>
+        <v>7252.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>46947.0</v>
+        <v>37712.0</v>
       </c>
       <c r="B52" t="n">
-        <v>35714.0</v>
+        <v>29165.0</v>
       </c>
       <c r="C52" t="n">
-        <v>5026.0</v>
+        <v>4457.0</v>
       </c>
       <c r="D52" t="n">
-        <v>167.0</v>
+        <v>136.0</v>
       </c>
       <c r="E52" t="n">
-        <v>11066.0</v>
+        <v>8411.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52361.0</v>
+        <v>42642.0</v>
       </c>
       <c r="B53" t="n">
-        <v>39398.0</v>
+        <v>32775.0</v>
       </c>
       <c r="C53" t="n">
-        <v>5414.0</v>
+        <v>4930.0</v>
       </c>
       <c r="D53" t="n">
-        <v>195.0</v>
+        <v>157.0</v>
       </c>
       <c r="E53" t="n">
-        <v>12768.0</v>
+        <v>9710.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>58002.0</v>
+        <v>48072.0</v>
       </c>
       <c r="B54" t="n">
-        <v>43049.0</v>
+        <v>36682.0</v>
       </c>
       <c r="C54" t="n">
-        <v>5641.0</v>
+        <v>5430.0</v>
       </c>
       <c r="D54" t="n">
-        <v>231.0</v>
+        <v>187.0</v>
       </c>
       <c r="E54" t="n">
-        <v>14722.0</v>
+        <v>11203.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>63879.0</v>
+        <v>54027.0</v>
       </c>
       <c r="B55" t="n">
-        <v>46732.0</v>
+        <v>40922.0</v>
       </c>
       <c r="C55" t="n">
-        <v>5877.0</v>
+        <v>5955.0</v>
       </c>
       <c r="D55" t="n">
-        <v>263.0</v>
+        <v>207.0</v>
       </c>
       <c r="E55" t="n">
-        <v>16884.0</v>
+        <v>12898.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>69906.0</v>
+        <v>60236.0</v>
       </c>
       <c r="B56" t="n">
-        <v>50238.0</v>
+        <v>45253.0</v>
       </c>
       <c r="C56" t="n">
-        <v>6027.0</v>
+        <v>6209.0</v>
       </c>
       <c r="D56" t="n">
-        <v>304.0</v>
+        <v>240.0</v>
       </c>
       <c r="E56" t="n">
-        <v>19364.0</v>
+        <v>14743.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>76270.0</v>
+        <v>67059.0</v>
       </c>
       <c r="B57" t="n">
-        <v>53988.0</v>
+        <v>49899.0</v>
       </c>
       <c r="C57" t="n">
-        <v>6364.0</v>
+        <v>6823.0</v>
       </c>
       <c r="D57" t="n">
-        <v>351.0</v>
+        <v>282.0</v>
       </c>
       <c r="E57" t="n">
-        <v>21931.0</v>
+        <v>16878.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>82708.0</v>
+        <v>74727.0</v>
       </c>
       <c r="B58" t="n">
-        <v>57360.0</v>
+        <v>55124.0</v>
       </c>
       <c r="C58" t="n">
-        <v>6438.0</v>
+        <v>7668.0</v>
       </c>
       <c r="D58" t="n">
-        <v>394.0</v>
+        <v>322.0</v>
       </c>
       <c r="E58" t="n">
-        <v>24954.0</v>
+        <v>19281.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>89373.0</v>
+        <v>82935.0</v>
       </c>
       <c r="B59" t="n">
-        <v>60794.0</v>
+        <v>60616.0</v>
       </c>
       <c r="C59" t="n">
-        <v>6665.0</v>
+        <v>8208.0</v>
       </c>
       <c r="D59" t="n">
-        <v>451.0</v>
+        <v>367.0</v>
       </c>
       <c r="E59" t="n">
-        <v>28128.0</v>
+        <v>21952.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>96128.0</v>
+        <v>92085.0</v>
       </c>
       <c r="B60" t="n">
-        <v>63980.0</v>
+        <v>66642.0</v>
       </c>
       <c r="C60" t="n">
-        <v>6755.0</v>
+        <v>9150.0</v>
       </c>
       <c r="D60" t="n">
-        <v>511.0</v>
+        <v>419.0</v>
       </c>
       <c r="E60" t="n">
-        <v>31637.0</v>
+        <v>25024.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>103160.0</v>
+        <v>102094.0</v>
       </c>
       <c r="B61" t="n">
-        <v>67105.0</v>
+        <v>73170.0</v>
       </c>
       <c r="C61" t="n">
-        <v>7032.0</v>
+        <v>10009.0</v>
       </c>
       <c r="D61" t="n">
-        <v>585.0</v>
+        <v>479.0</v>
       </c>
       <c r="E61" t="n">
-        <v>35470.0</v>
+        <v>28445.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>110221.0</v>
+        <v>113183.0</v>
       </c>
       <c r="B62" t="n">
-        <v>70000.0</v>
+        <v>80584.0</v>
       </c>
       <c r="C62" t="n">
-        <v>7061.0</v>
+        <v>11089.0</v>
       </c>
       <c r="D62" t="n">
-        <v>666.0</v>
+        <v>525.0</v>
       </c>
       <c r="E62" t="n">
-        <v>39555.0</v>
+        <v>32074.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>117523.0</v>
+        <v>125309.0</v>
       </c>
       <c r="B63" t="n">
-        <v>72805.0</v>
+        <v>88522.0</v>
       </c>
       <c r="C63" t="n">
-        <v>7302.0</v>
+        <v>12126.0</v>
       </c>
       <c r="D63" t="n">
-        <v>742.0</v>
+        <v>604.0</v>
       </c>
       <c r="E63" t="n">
-        <v>43976.0</v>
+        <v>36183.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>124886.0</v>
+        <v>138840.0</v>
       </c>
       <c r="B64" t="n">
-        <v>75316.0</v>
+        <v>97360.0</v>
       </c>
       <c r="C64" t="n">
-        <v>7363.0</v>
+        <v>13531.0</v>
       </c>
       <c r="D64" t="n">
-        <v>823.0</v>
+        <v>687.0</v>
       </c>
       <c r="E64" t="n">
-        <v>48747.0</v>
+        <v>40793.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>132177.0</v>
+        <v>153582.0</v>
       </c>
       <c r="B65" t="n">
-        <v>77613.0</v>
+        <v>107064.0</v>
       </c>
       <c r="C65" t="n">
-        <v>7291.0</v>
+        <v>14742.0</v>
       </c>
       <c r="D65" t="n">
-        <v>920.0</v>
+        <v>775.0</v>
       </c>
       <c r="E65" t="n">
-        <v>53644.0</v>
+        <v>45743.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>139531.0</v>
+        <v>169890.0</v>
       </c>
       <c r="B66" t="n">
-        <v>79656.0</v>
+        <v>117798.0</v>
       </c>
       <c r="C66" t="n">
-        <v>7354.0</v>
+        <v>16308.0</v>
       </c>
       <c r="D66" t="n">
-        <v>1005.0</v>
+        <v>871.0</v>
       </c>
       <c r="E66" t="n">
-        <v>58870.0</v>
+        <v>51221.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>147027.0</v>
+        <v>187910.0</v>
       </c>
       <c r="B67" t="n">
-        <v>81499.0</v>
+        <v>129698.0</v>
       </c>
       <c r="C67" t="n">
-        <v>7496.0</v>
+        <v>18020.0</v>
       </c>
       <c r="D67" t="n">
-        <v>1129.0</v>
+        <v>968.0</v>
       </c>
       <c r="E67" t="n">
-        <v>64399.0</v>
+        <v>57244.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>154407.0</v>
+        <v>207463.0</v>
       </c>
       <c r="B68" t="n">
-        <v>82984.0</v>
+        <v>142458.0</v>
       </c>
       <c r="C68" t="n">
-        <v>7380.0</v>
+        <v>19553.0</v>
       </c>
       <c r="D68" t="n">
-        <v>1251.0</v>
+        <v>1072.0</v>
       </c>
       <c r="E68" t="n">
-        <v>70172.0</v>
+        <v>63933.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>161824.0</v>
+        <v>228632.0</v>
       </c>
       <c r="B69" t="n">
-        <v>84385.0</v>
+        <v>156246.0</v>
       </c>
       <c r="C69" t="n">
-        <v>7417.0</v>
+        <v>21169.0</v>
       </c>
       <c r="D69" t="n">
-        <v>1343.0</v>
+        <v>1196.0</v>
       </c>
       <c r="E69" t="n">
-        <v>76096.0</v>
+        <v>71190.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>169307.0</v>
+        <v>251247.0</v>
       </c>
       <c r="B70" t="n">
-        <v>85665.0</v>
+        <v>170748.0</v>
       </c>
       <c r="C70" t="n">
-        <v>7483.0</v>
+        <v>22615.0</v>
       </c>
       <c r="D70" t="n">
-        <v>1471.0</v>
+        <v>1320.0</v>
       </c>
       <c r="E70" t="n">
-        <v>82171.0</v>
+        <v>79179.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>176745.0</v>
+        <v>275073.0</v>
       </c>
       <c r="B71" t="n">
-        <v>86590.0</v>
+        <v>185754.0</v>
       </c>
       <c r="C71" t="n">
-        <v>7438.0</v>
+        <v>23826.0</v>
       </c>
       <c r="D71" t="n">
-        <v>1582.0</v>
+        <v>1446.0</v>
       </c>
       <c r="E71" t="n">
-        <v>88573.0</v>
+        <v>87873.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>184008.0</v>
+        <v>301328.0</v>
       </c>
       <c r="B72" t="n">
-        <v>87345.0</v>
+        <v>202200.0</v>
       </c>
       <c r="C72" t="n">
-        <v>7263.0</v>
+        <v>26255.0</v>
       </c>
       <c r="D72" t="n">
-        <v>1695.0</v>
+        <v>1622.0</v>
       </c>
       <c r="E72" t="n">
-        <v>94968.0</v>
+        <v>97506.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>191197.0</v>
+        <v>329381.0</v>
       </c>
       <c r="B73" t="n">
-        <v>87831.0</v>
+        <v>219464.0</v>
       </c>
       <c r="C73" t="n">
-        <v>7189.0</v>
+        <v>28053.0</v>
       </c>
       <c r="D73" t="n">
-        <v>1802.0</v>
+        <v>1783.0</v>
       </c>
       <c r="E73" t="n">
-        <v>101564.0</v>
+        <v>108134.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>198292.0</v>
+        <v>358398.0</v>
       </c>
       <c r="B74" t="n">
-        <v>88063.0</v>
+        <v>236828.0</v>
       </c>
       <c r="C74" t="n">
-        <v>7095.0</v>
+        <v>29017.0</v>
       </c>
       <c r="D74" t="n">
-        <v>1936.0</v>
+        <v>1962.0</v>
       </c>
       <c r="E74" t="n">
-        <v>108293.0</v>
+        <v>119608.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>205245.0</v>
+        <v>389495.0</v>
       </c>
       <c r="B75" t="n">
-        <v>88251.0</v>
+        <v>254947.0</v>
       </c>
       <c r="C75" t="n">
-        <v>6953.0</v>
+        <v>31097.0</v>
       </c>
       <c r="D75" t="n">
-        <v>2073.0</v>
+        <v>2167.0</v>
       </c>
       <c r="E75" t="n">
-        <v>114921.0</v>
+        <v>132381.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>212011.0</v>
+        <v>421399.0</v>
       </c>
       <c r="B76" t="n">
-        <v>88087.0</v>
+        <v>272668.0</v>
       </c>
       <c r="C76" t="n">
-        <v>6766.0</v>
+        <v>31904.0</v>
       </c>
       <c r="D76" t="n">
-        <v>2197.0</v>
+        <v>2401.0</v>
       </c>
       <c r="E76" t="n">
-        <v>121727.0</v>
+        <v>146330.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>218613.0</v>
+        <v>454897.0</v>
       </c>
       <c r="B77" t="n">
-        <v>87716.0</v>
+        <v>290642.0</v>
       </c>
       <c r="C77" t="n">
-        <v>6602.0</v>
+        <v>33498.0</v>
       </c>
       <c r="D77" t="n">
-        <v>2334.0</v>
+        <v>2651.0</v>
       </c>
       <c r="E77" t="n">
-        <v>128563.0</v>
+        <v>161604.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>225077.0</v>
+        <v>489320.0</v>
       </c>
       <c r="B78" t="n">
-        <v>87118.0</v>
+        <v>308391.0</v>
       </c>
       <c r="C78" t="n">
-        <v>6464.0</v>
+        <v>34423.0</v>
       </c>
       <c r="D78" t="n">
-        <v>2467.0</v>
+        <v>2942.0</v>
       </c>
       <c r="E78" t="n">
-        <v>135492.0</v>
+        <v>177987.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>231294.0</v>
+        <v>524430.0</v>
       </c>
       <c r="B79" t="n">
-        <v>86096.0</v>
+        <v>325033.0</v>
       </c>
       <c r="C79" t="n">
-        <v>6217.0</v>
+        <v>35110.0</v>
       </c>
       <c r="D79" t="n">
-        <v>2578.0</v>
+        <v>3243.0</v>
       </c>
       <c r="E79" t="n">
-        <v>142620.0</v>
+        <v>196154.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>237502.0</v>
+        <v>560998.0</v>
       </c>
       <c r="B80" t="n">
-        <v>85076.0</v>
+        <v>341563.0</v>
       </c>
       <c r="C80" t="n">
-        <v>6208.0</v>
+        <v>36568.0</v>
       </c>
       <c r="D80" t="n">
-        <v>2713.0</v>
+        <v>3589.0</v>
       </c>
       <c r="E80" t="n">
-        <v>149713.0</v>
+        <v>215846.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>243636.0</v>
+        <v>597765.0</v>
       </c>
       <c r="B81" t="n">
-        <v>84006.0</v>
+        <v>356961.0</v>
       </c>
       <c r="C81" t="n">
-        <v>6134.0</v>
+        <v>36767.0</v>
       </c>
       <c r="D81" t="n">
-        <v>2841.0</v>
+        <v>3937.0</v>
       </c>
       <c r="E81" t="n">
-        <v>156789.0</v>
+        <v>236867.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>249759.0</v>
+        <v>634944.0</v>
       </c>
       <c r="B82" t="n">
-        <v>83002.0</v>
+        <v>371524.0</v>
       </c>
       <c r="C82" t="n">
-        <v>6123.0</v>
+        <v>37179.0</v>
       </c>
       <c r="D82" t="n">
-        <v>2972.0</v>
+        <v>4289.0</v>
       </c>
       <c r="E82" t="n">
-        <v>163785.0</v>
+        <v>259131.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>255721.0</v>
+        <v>672627.0</v>
       </c>
       <c r="B83" t="n">
-        <v>81926.0</v>
+        <v>385130.0</v>
       </c>
       <c r="C83" t="n">
-        <v>5962.0</v>
+        <v>37683.0</v>
       </c>
       <c r="D83" t="n">
-        <v>3090.0</v>
+        <v>4721.0</v>
       </c>
       <c r="E83" t="n">
-        <v>170705.0</v>
+        <v>282776.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>261311.0</v>
+        <v>710082.0</v>
       </c>
       <c r="B84" t="n">
-        <v>80597.0</v>
+        <v>397000.0</v>
       </c>
       <c r="C84" t="n">
-        <v>5590.0</v>
+        <v>37455.0</v>
       </c>
       <c r="D84" t="n">
-        <v>3234.0</v>
+        <v>5177.0</v>
       </c>
       <c r="E84" t="n">
-        <v>177480.0</v>
+        <v>307905.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>266843.0</v>
+        <v>747271.0</v>
       </c>
       <c r="B85" t="n">
-        <v>79053.0</v>
+        <v>407372.0</v>
       </c>
       <c r="C85" t="n">
-        <v>5532.0</v>
+        <v>37189.0</v>
       </c>
       <c r="D85" t="n">
-        <v>3364.0</v>
+        <v>5719.0</v>
       </c>
       <c r="E85" t="n">
-        <v>184426.0</v>
+        <v>334180.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>272179.0</v>
+        <v>783915.0</v>
       </c>
       <c r="B86" t="n">
-        <v>77538.0</v>
+        <v>415831.0</v>
       </c>
       <c r="C86" t="n">
-        <v>5336.0</v>
+        <v>36644.0</v>
       </c>
       <c r="D86" t="n">
-        <v>3466.0</v>
+        <v>6213.0</v>
       </c>
       <c r="E86" t="n">
-        <v>191175.0</v>
+        <v>361871.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>277325.0</v>
+        <v>820757.0</v>
       </c>
       <c r="B87" t="n">
-        <v>75950.0</v>
+        <v>423176.0</v>
       </c>
       <c r="C87" t="n">
-        <v>5146.0</v>
+        <v>36842.0</v>
       </c>
       <c r="D87" t="n">
-        <v>3590.0</v>
+        <v>6740.0</v>
       </c>
       <c r="E87" t="n">
-        <v>197785.0</v>
+        <v>390841.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>282471.0</v>
+        <v>856661.0</v>
       </c>
       <c r="B88" t="n">
-        <v>74500.0</v>
+        <v>428249.0</v>
       </c>
       <c r="C88" t="n">
-        <v>5146.0</v>
+        <v>35904.0</v>
       </c>
       <c r="D88" t="n">
-        <v>3694.0</v>
+        <v>7258.0</v>
       </c>
       <c r="E88" t="n">
-        <v>204277.0</v>
+        <v>421154.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>287600.0</v>
+        <v>891842.0</v>
       </c>
       <c r="B89" t="n">
-        <v>73027.0</v>
+        <v>431859.0</v>
       </c>
       <c r="C89" t="n">
-        <v>5129.0</v>
+        <v>35181.0</v>
       </c>
       <c r="D89" t="n">
-        <v>3811.0</v>
+        <v>7783.0</v>
       </c>
       <c r="E89" t="n">
-        <v>210762.0</v>
+        <v>452200.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>292334.0</v>
+        <v>926469.0</v>
       </c>
       <c r="B90" t="n">
-        <v>71312.0</v>
+        <v>433792.0</v>
       </c>
       <c r="C90" t="n">
-        <v>4734.0</v>
+        <v>34627.0</v>
       </c>
       <c r="D90" t="n">
-        <v>3920.0</v>
+        <v>8366.0</v>
       </c>
       <c r="E90" t="n">
-        <v>217102.0</v>
+        <v>484311.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>297031.0</v>
+        <v>959711.0</v>
       </c>
       <c r="B91" t="n">
-        <v>69609.0</v>
+        <v>433522.0</v>
       </c>
       <c r="C91" t="n">
-        <v>4697.0</v>
+        <v>33242.0</v>
       </c>
       <c r="D91" t="n">
-        <v>4023.0</v>
+        <v>8978.0</v>
       </c>
       <c r="E91" t="n">
-        <v>223399.0</v>
+        <v>517211.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>301437.0</v>
+        <v>991729.0</v>
       </c>
       <c r="B92" t="n">
-        <v>67829.0</v>
+        <v>431244.0</v>
       </c>
       <c r="C92" t="n">
-        <v>4406.0</v>
+        <v>32018.0</v>
       </c>
       <c r="D92" t="n">
-        <v>4122.0</v>
+        <v>9597.0</v>
       </c>
       <c r="E92" t="n">
-        <v>229486.0</v>
+        <v>550888.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>305806.0</v>
+        <v>1022683.0</v>
       </c>
       <c r="B93" t="n">
-        <v>66125.0</v>
+        <v>427405.0</v>
       </c>
       <c r="C93" t="n">
-        <v>4369.0</v>
+        <v>30954.0</v>
       </c>
       <c r="D93" t="n">
-        <v>4217.0</v>
+        <v>10253.0</v>
       </c>
       <c r="E93" t="n">
-        <v>235464.0</v>
+        <v>585025.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>310112.0</v>
+        <v>1052306.0</v>
       </c>
       <c r="B94" t="n">
-        <v>64506.0</v>
+        <v>421460.0</v>
       </c>
       <c r="C94" t="n">
-        <v>4306.0</v>
+        <v>29623.0</v>
       </c>
       <c r="D94" t="n">
-        <v>4310.0</v>
+        <v>10914.0</v>
       </c>
       <c r="E94" t="n">
-        <v>241296.0</v>
+        <v>619932.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>314208.0</v>
+        <v>1080569.0</v>
       </c>
       <c r="B95" t="n">
-        <v>62769.0</v>
+        <v>414351.0</v>
       </c>
       <c r="C95" t="n">
-        <v>4096.0</v>
+        <v>28263.0</v>
       </c>
       <c r="D95" t="n">
-        <v>4414.0</v>
+        <v>11569.0</v>
       </c>
       <c r="E95" t="n">
-        <v>247025.0</v>
+        <v>654649.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>318323.0</v>
+        <v>1107559.0</v>
       </c>
       <c r="B96" t="n">
-        <v>61101.0</v>
+        <v>405885.0</v>
       </c>
       <c r="C96" t="n">
-        <v>4115.0</v>
+        <v>26990.0</v>
       </c>
       <c r="D96" t="n">
-        <v>4503.0</v>
+        <v>12213.0</v>
       </c>
       <c r="E96" t="n">
-        <v>252719.0</v>
+        <v>689461.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>322109.0</v>
+        <v>1132967.0</v>
       </c>
       <c r="B97" t="n">
-        <v>59361.0</v>
+        <v>395732.0</v>
       </c>
       <c r="C97" t="n">
-        <v>3786.0</v>
+        <v>25408.0</v>
       </c>
       <c r="D97" t="n">
-        <v>4595.0</v>
+        <v>12852.0</v>
       </c>
       <c r="E97" t="n">
-        <v>258153.0</v>
+        <v>724383.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>325795.0</v>
+        <v>1156439.0</v>
       </c>
       <c r="B98" t="n">
-        <v>57579.0</v>
+        <v>384374.0</v>
       </c>
       <c r="C98" t="n">
-        <v>3686.0</v>
+        <v>23472.0</v>
       </c>
       <c r="D98" t="n">
-        <v>4680.0</v>
+        <v>13502.0</v>
       </c>
       <c r="E98" t="n">
-        <v>263536.0</v>
+        <v>758563.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>329324.0</v>
+        <v>1178454.0</v>
       </c>
       <c r="B99" t="n">
-        <v>55700.0</v>
+        <v>371228.0</v>
       </c>
       <c r="C99" t="n">
-        <v>3529.0</v>
+        <v>22015.0</v>
       </c>
       <c r="D99" t="n">
-        <v>4786.0</v>
+        <v>14159.0</v>
       </c>
       <c r="E99" t="n">
-        <v>268838.0</v>
+        <v>793067.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>332785.0</v>
+        <v>1198862.0</v>
       </c>
       <c r="B100" t="n">
-        <v>54197.0</v>
+        <v>357712.0</v>
       </c>
       <c r="C100" t="n">
-        <v>3461.0</v>
+        <v>20408.0</v>
       </c>
       <c r="D100" t="n">
-        <v>4868.0</v>
+        <v>14788.0</v>
       </c>
       <c r="E100" t="n">
-        <v>273720.0</v>
+        <v>826362.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>336128.0</v>
+        <v>1217703.0</v>
       </c>
       <c r="B101" t="n">
-        <v>52576.0</v>
+        <v>343254.0</v>
       </c>
       <c r="C101" t="n">
-        <v>3343.0</v>
+        <v>18841.0</v>
       </c>
       <c r="D101" t="n">
-        <v>4944.0</v>
+        <v>15371.0</v>
       </c>
       <c r="E101" t="n">
-        <v>278608.0</v>
+        <v>859078.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>339317.0</v>
+        <v>1235351.0</v>
       </c>
       <c r="B102" t="n">
-        <v>50963.0</v>
+        <v>328314.0</v>
       </c>
       <c r="C102" t="n">
-        <v>3189.0</v>
+        <v>17648.0</v>
       </c>
       <c r="D102" t="n">
-        <v>5026.0</v>
+        <v>15966.0</v>
       </c>
       <c r="E102" t="n">
-        <v>283328.0</v>
+        <v>891071.0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>342356.0</v>
+        <v>1251647.0</v>
       </c>
       <c r="B103" t="n">
-        <v>49280.0</v>
+        <v>312660.0</v>
       </c>
       <c r="C103" t="n">
-        <v>3039.0</v>
+        <v>16296.0</v>
       </c>
       <c r="D103" t="n">
-        <v>5094.0</v>
+        <v>16542.0</v>
       </c>
       <c r="E103" t="n">
-        <v>287982.0</v>
+        <v>922445.0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>345246.0</v>
+        <v>1266913.0</v>
       </c>
       <c r="B104" t="n">
-        <v>47606.0</v>
+        <v>297006.0</v>
       </c>
       <c r="C104" t="n">
-        <v>2890.0</v>
+        <v>15266.0</v>
       </c>
       <c r="D104" t="n">
-        <v>5167.0</v>
+        <v>17064.0</v>
       </c>
       <c r="E104" t="n">
-        <v>292473.0</v>
+        <v>952843.0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>348028.0</v>
+        <v>1280740.0</v>
       </c>
       <c r="B105" t="n">
-        <v>45812.0</v>
+        <v>281366.0</v>
       </c>
       <c r="C105" t="n">
-        <v>2782.0</v>
+        <v>13827.0</v>
       </c>
       <c r="D105" t="n">
-        <v>5248.0</v>
+        <v>17545.0</v>
       </c>
       <c r="E105" t="n">
-        <v>296968.0</v>
+        <v>981829.0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>350800.0</v>
+        <v>1293477.0</v>
       </c>
       <c r="B106" t="n">
-        <v>44358.0</v>
+        <v>265663.0</v>
       </c>
       <c r="C106" t="n">
-        <v>2772.0</v>
+        <v>12737.0</v>
       </c>
       <c r="D106" t="n">
-        <v>5311.0</v>
+        <v>18034.0</v>
       </c>
       <c r="E106" t="n">
-        <v>301131.0</v>
+        <v>1009780.0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>353557.0</v>
+        <v>1304920.0</v>
       </c>
       <c r="B107" t="n">
-        <v>42963.0</v>
+        <v>249804.0</v>
       </c>
       <c r="C107" t="n">
-        <v>2757.0</v>
+        <v>11443.0</v>
       </c>
       <c r="D107" t="n">
-        <v>5373.0</v>
+        <v>18512.0</v>
       </c>
       <c r="E107" t="n">
-        <v>305221.0</v>
+        <v>1036604.0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>356097.0</v>
+        <v>1315541.0</v>
       </c>
       <c r="B108" t="n">
-        <v>41524.0</v>
+        <v>234450.0</v>
       </c>
       <c r="C108" t="n">
-        <v>2540.0</v>
+        <v>10621.0</v>
       </c>
       <c r="D108" t="n">
-        <v>5437.0</v>
+        <v>18997.0</v>
       </c>
       <c r="E108" t="n">
-        <v>309136.0</v>
+        <v>1062094.0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>358642.0</v>
+        <v>1325352.0</v>
       </c>
       <c r="B109" t="n">
-        <v>40199.0</v>
+        <v>219703.0</v>
       </c>
       <c r="C109" t="n">
-        <v>2545.0</v>
+        <v>9811.0</v>
       </c>
       <c r="D109" t="n">
-        <v>5496.0</v>
+        <v>19421.0</v>
       </c>
       <c r="E109" t="n">
-        <v>312947.0</v>
+        <v>1086228.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>